<commit_message>
Updated kinetic parameters from Enguang
</commit_message>
<xml_diff>
--- a/input_data/kinetic_params.xlsx
+++ b/input_data/kinetic_params.xlsx
@@ -4833,7 +4833,7 @@
       <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.33"/>
@@ -8117,7 +8117,7 @@
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.84"/>
@@ -31852,8 +31852,8 @@
   </sheetPr>
   <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.87890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -31906,7 +31906,7 @@
         <v>806</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>6000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32170,7 +32170,7 @@
         <v>806</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>3900</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32181,7 +32181,7 @@
         <v>807</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>310</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32258,7 +32258,7 @@
         <v>806</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>1.72</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>